<commit_message>
Add Google Drive link conversion utility and update embedder to use direct download links; remove unused retriever engine
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -16,20 +16,20 @@
     <t>urls</t>
   </si>
   <si>
-    <t>https://lpi.oregonstate.edu/sites/lpi.oregonstate.edu/files/pdf/mic/micronutrients_for_health.pdf</t>
+    <t>https://drive.google.com/file/d/1ntkwGeHmmkyQXtEuP3yIC_zfeDbyVvNt/view?usp=sharing</t>
   </si>
   <si>
-    <t>https://www.accessdata.fda.gov/scripts/InteractiveNutritionFactsLabel/assets/InteractiveNFL_Vitamins%26MineralsChart_October2021.pdf</t>
+    <t>https://drive.google.com/file/d/1ncu7OPrXB2i3nV6TWJjohSSHzcy2tYDL/view?usp=sharing</t>
   </si>
   <si>
-    <t>https://www.hilarispublisher.com/open-access/essential-nutrients-in-human-body.pdf</t>
+    <t>https://drive.google.com/file/d/199F9gjwuSCNRCSZoakqSIxVRWmCOfNoT/view?usp=sharing</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -40,10 +40,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <color rgb="FF0000FF"/>
     </font>
     <font>
       <u/>
@@ -64,7 +60,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -72,9 +68,6 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -292,6 +285,9 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="70.63"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -309,7 +305,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>